<commit_message>
Mejorar manejo de respuestas del backend - mostrar conteo de propiedades
</commit_message>
<xml_diff>
--- a/propiedades.xlsx
+++ b/propiedades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artar\Downloads\CHATGPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53CD466-C55A-464D-AC87-C1EC42B78245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D05C1A5-2179-42FE-B877-E4C3A5B6AF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1845,7 +1845,7 @@
         <v>137</v>
       </c>
       <c r="B17" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="C17">
         <v>600000</v>

</xml_diff>

<commit_message>
Feat: Crear prompt específico para preguntas de seguimiento con todos los detalles de propiedades
</commit_message>
<xml_diff>
--- a/propiedades.xlsx
+++ b/propiedades.xlsx
@@ -8,14 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artar\Downloads\CHATGPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D05C1A5-2179-42FE-B877-E4C3A5B6AF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02D32EE-9255-4C2F-8F87-9C96F2EDA190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$U$17</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -797,10 +813,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -942,7 +959,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1134,7 +1151,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1199,7 +1216,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -1326,7 +1343,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -1456,7 +1473,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -1713,7 +1730,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -1775,7 +1792,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>127</v>
       </c>
@@ -1840,7 +1857,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>137</v>
       </c>
@@ -1906,6 +1923,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U17" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="alquiler"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: corrección carga propiedades y detección de filtros
</commit_message>
<xml_diff>
--- a/propiedades.xlsx
+++ b/propiedades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artar\Downloads\CHATGPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DB1BAB-A7BA-48CA-BB2D-50EE9F78C4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BB4B57-BF14-4267-B6CE-4FB4429AC1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="139">
   <si>
     <t>titulo</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>Terreno en Boedo, para desarrollo</t>
+  </si>
+  <si>
+    <t>Exclusivo terreno apto para desarrollo inmobiliario</t>
   </si>
 </sst>
 </file>
@@ -816,13 +819,14 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:U1"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.90625" customWidth="1"/>
     <col min="9" max="9" width="24.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.26953125" customWidth="1"/>
     <col min="15" max="15" width="50" bestFit="1" customWidth="1"/>
@@ -1879,7 +1883,7 @@
         <v>134</v>
       </c>
       <c r="H17" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="I17" t="s">
         <v>135</v>

</xml_diff>